<commit_message>
do UI. Rename find element: _by_
</commit_message>
<xml_diff>
--- a/new_verst_11_11/123.xlsx
+++ b/new_verst_11_11/123.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\TIC\sch-20200301T104329Z-001\New K WB\selenium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\pycharm projects\selenium\retailsys\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="71">
   <si>
     <t>#מזהה מכירה</t>
   </si>
@@ -240,10 +240,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -321,7 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -342,8 +339,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -359,9 +356,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -399,7 +396,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -471,7 +468,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -648,31 +645,31 @@
   <sheetPr>
     <tabColor rgb="FF4285F4"/>
   </sheetPr>
-  <dimension ref="A1:BF2"/>
+  <dimension ref="A1:BF5"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="15" customWidth="1"/>
-    <col min="17" max="17" width="35.5703125" customWidth="1"/>
+    <col min="17" max="17" width="35.5546875" customWidth="1"/>
     <col min="18" max="21" width="15" customWidth="1"/>
-    <col min="22" max="22" width="37.7109375" customWidth="1"/>
+    <col min="22" max="22" width="37.6640625" customWidth="1"/>
     <col min="23" max="41" width="15" customWidth="1"/>
     <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -842,7 +839,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>226687</v>
       </c>
@@ -970,6 +967,390 @@
       </c>
       <c r="BF2" s="1"/>
     </row>
+    <row r="3" spans="1:58" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>226687</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
+        <v>343182333</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="1">
+        <v>489391</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>44465</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>526476088</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO3" s="1">
+        <v>1231231321</v>
+      </c>
+      <c r="AP3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+      <c r="AX3" s="1"/>
+      <c r="AY3" s="1"/>
+      <c r="AZ3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB3" s="1"/>
+      <c r="BC3" s="1"/>
+      <c r="BD3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BF3" s="1"/>
+    </row>
+    <row r="4" spans="1:58" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>226687</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
+        <v>343182333</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="1">
+        <v>489391</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>44465</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>526476088</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO4" s="1">
+        <v>1231231321</v>
+      </c>
+      <c r="AP4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="1"/>
+      <c r="AW4" s="1"/>
+      <c r="AX4" s="1"/>
+      <c r="AY4" s="1"/>
+      <c r="AZ4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB4" s="1"/>
+      <c r="BC4" s="1"/>
+      <c r="BD4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BE4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BF4" s="1"/>
+    </row>
+    <row r="5" spans="1:58" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>226687</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>343182333</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="1">
+        <v>489391</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>44465</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>526476088</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO5" s="1">
+        <v>1231231321</v>
+      </c>
+      <c r="AP5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="1"/>
+      <c r="AW5" s="1"/>
+      <c r="AX5" s="1"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BA5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB5" s="1"/>
+      <c r="BC5" s="1"/>
+      <c r="BD5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BE5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BF5" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>